<commit_message>
case 2 3 4
</commit_message>
<xml_diff>
--- a/case1.xlsx
+++ b/case1.xlsx
@@ -8,135 +8,257 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroGrids\Documents\Ofun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EF1F02-A1C0-4101-824A-2B752A30866C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D74EC-D71C-4423-9B5A-E8C332675753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" activeTab="1" xr2:uid="{112FC91A-F7FB-432D-9E1C-6D1B5AB132A1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" activeTab="3" xr2:uid="{112FC91A-F7FB-432D-9E1C-6D1B5AB132A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Case1a" sheetId="1" r:id="rId1"/>
     <sheet name="Case1b" sheetId="3" r:id="rId2"/>
+    <sheet name="Case1c" sheetId="4" r:id="rId3"/>
+    <sheet name="Case1d" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Case1a!$B$10:$G$15</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Case1b!$B$10:$G$15</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Case1c!$L$35:$T$43,Case1c!$R$33:$T$33</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Case1d!$L$35:$T$43,Case1d!$R$33:$T$33,Case1d!$E$2:$E$7</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Case1a!$A$23:$A$28</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Case1b!$A$23:$A$28</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Case1c!$A$19:$A$27</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Case1d!$A$19:$A$27</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">Case1a!$G$16</definedName>
     <definedName name="solver_lhs10" localSheetId="1" hidden="1">Case1b!$H$15</definedName>
+    <definedName name="solver_lhs10" localSheetId="2" hidden="1">Case1c!$U$35:$U$40</definedName>
+    <definedName name="solver_lhs10" localSheetId="3" hidden="1">Case1d!$U$33</definedName>
     <definedName name="solver_lhs11" localSheetId="0" hidden="1">Case1a!$H$15</definedName>
     <definedName name="solver_lhs11" localSheetId="1" hidden="1">Case1b!$H$15</definedName>
+    <definedName name="solver_lhs11" localSheetId="2" hidden="1">Case1c!$U$41:$U$43</definedName>
+    <definedName name="solver_lhs11" localSheetId="3" hidden="1">Case1d!$U$41:$U$43</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Case1a!$B$10:$G$15</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Case1b!$B$10:$G$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Case1c!$C$30</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Case1d!$C$30:$C$44</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Case1a!$B$16</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Case1b!$B$16:$C$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Case1c!$L$35:$T$43</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Case1d!$E$2:$E$7</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Case1a!$C$16:$F$16</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">Case1b!$C$30:$C$35</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">Case1c!$L$44:$O$44</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Case1d!$L$35:$T$43</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Case1a!$C$30:$C$35</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">Case1b!$D$16:$F$16</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">Case1c!$P$44:$Q$44</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Case1d!$L$44:$Q$44</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">Case1a!$G$10</definedName>
     <definedName name="solver_lhs6" localSheetId="1" hidden="1">Case1b!$G$16</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">Case1c!$R$33:$T$33</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">Case1d!$R$33:$T$33</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">Case1a!$G$16</definedName>
     <definedName name="solver_lhs7" localSheetId="1" hidden="1">Case1b!$G$30</definedName>
+    <definedName name="solver_lhs7" localSheetId="2" hidden="1">Case1c!$R$44:$T$44</definedName>
+    <definedName name="solver_lhs7" localSheetId="3" hidden="1">Case1d!$R$44:$T$44</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">Case1a!$H$10:$H$14</definedName>
     <definedName name="solver_lhs8" localSheetId="1" hidden="1">Case1b!$H$10:$H$14</definedName>
+    <definedName name="solver_lhs8" localSheetId="2" hidden="1">Case1c!$R$48:$T$48</definedName>
+    <definedName name="solver_lhs8" localSheetId="3" hidden="1">Case1d!$R$6</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">Case1a!$H$15</definedName>
     <definedName name="solver_lhs9" localSheetId="1" hidden="1">Case1b!$H$15</definedName>
+    <definedName name="solver_lhs9" localSheetId="2" hidden="1">Case1c!$U$33</definedName>
+    <definedName name="solver_lhs9" localSheetId="3" hidden="1">Case1d!$R$6</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">9</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">9</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">11</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">10</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Case1a!$I$1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Case1b!$G$30</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Case1b!$N$1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Case1c!$R$1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Case1d!$R$1</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel10" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel10" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel11" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel11" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel11" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel8" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel9" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel9" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel9" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs10" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs10" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs10" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs11" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs11" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs11" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs11" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">binaire</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">binaire</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">binaire</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">binaire</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">binaire</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">Case1d!$L$50:$Q$50</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">Case1b!$N$6</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">binaire</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">binaire</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs7" localSheetId="1" hidden="1">Case1b!$N$8</definedName>
+    <definedName name="solver_rhs7" localSheetId="2" hidden="1">Case1c!$R$32:$T$32</definedName>
+    <definedName name="solver_rhs7" localSheetId="3" hidden="1">Case1d!$R$32:$T$32</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs8" localSheetId="2" hidden="1">Case1c!$R$8</definedName>
+    <definedName name="solver_rhs8" localSheetId="3" hidden="1">Case1d!$R$5</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs9" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs9" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs9" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -153,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="61">
   <si>
     <t>distance matrix</t>
   </si>
@@ -273,6 +395,69 @@
   </si>
   <si>
     <t>Condition départ-&gt;destination &lt;= Nv - Const</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>N points</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>Où je suis : S1</t>
+  </si>
+  <si>
+    <t>Où je vais:  S1</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Où je vais:  1</t>
+  </si>
+  <si>
+    <t>Où je suis : 1</t>
+  </si>
+  <si>
+    <t>activation voiture</t>
+  </si>
+  <si>
+    <t>1 - aj</t>
+  </si>
+  <si>
+    <t>sum aibij</t>
   </si>
 </sst>
 </file>
@@ -294,7 +479,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +522,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -350,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -359,11 +568,35 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -411,6 +644,104 @@
     <tableColumn id="1" xr3:uid="{7BB12CE3-74CF-436E-8A17-F1A5178B7ECC}" name="Coordonnées"/>
     <tableColumn id="2" xr3:uid="{415DC325-7992-41C2-B458-6FAE5A0E6D6E}" name="x"/>
     <tableColumn id="3" xr3:uid="{F0FBBDF7-9D25-443A-9CD7-865FC6601963}" name="y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{43277BFF-0245-4469-9CA5-75C0D84097BA}" name="Tableau22" displayName="Tableau22" ref="F1:O10" totalsRowShown="0">
+  <autoFilter ref="F1:O10" xr:uid="{4706B194-EB46-4EE1-B9C3-ED64E3DBE6C0}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{14688EF5-8275-4B93-899E-CEAF2EEE8845}" name="distance matrix"/>
+    <tableColumn id="2" xr3:uid="{CDC121EA-E7B2-43B3-B756-F7894E7E2A1B}" name="S1">
+      <calculatedColumnFormula>SQRT((C$2-C2)^2+(D$2-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{540F7FFB-D9F8-4AC8-901C-936701A5BB65}" name="S2">
+      <calculatedColumnFormula>SQRT((C$3-C2)^2+(D$3-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{439F6117-705F-4364-858C-FF856C173398}" name="S3">
+      <calculatedColumnFormula>SQRT((C$4-C2)^2+(D$4-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E432533C-A813-4CC9-BCE7-894891D33251}" name="S4">
+      <calculatedColumnFormula>SQRT((C$5-C2)^2+(D$5-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{BBB216F3-F863-4815-9975-8291E90562B1}" name="1">
+      <calculatedColumnFormula>SQRT((C$6-C2)^2+(D$6-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{04AF1A80-3A08-4309-B619-00461709794F}" name="2">
+      <calculatedColumnFormula>SQRT((C$7-C2)^2+(D$7-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{A4ECE921-FAD5-42E4-9E8A-CD14FF0225F6}" name="D1" dataDxfId="5">
+      <calculatedColumnFormula>SQRT((C$8-C2)^2+(D$8-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{E4050388-FB48-477D-91CC-9E49185CCD01}" name="D2" dataDxfId="4">
+      <calculatedColumnFormula>SQRT((C$9-C2)^2+(D$9-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{891843E9-97CB-41ED-B395-57529484DF73}" name="D3" dataDxfId="3">
+      <calculatedColumnFormula>SQRT((C$10-C2)^2+(D$10-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2F7C2CDB-ACD4-4C59-B9D2-1C5DB18D37C0}" name="Tableau35" displayName="Tableau35" ref="B1:D10" totalsRowShown="0">
+  <autoFilter ref="B1:D10" xr:uid="{23FEA744-B7A0-4AB4-BA8E-3D1EC4BABB72}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5CF40F08-CFD0-4BF1-A429-CD3449146525}" name="Coordonnées"/>
+    <tableColumn id="2" xr3:uid="{31B106F7-E477-47CE-8961-9D097D8018E4}" name="x"/>
+    <tableColumn id="3" xr3:uid="{CEDF20E8-47B1-43CE-B1C4-2ACB302610A4}" name="y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{3D0D121D-20C4-4250-A7D3-489F79C8CD6F}" name="Tableau2210" displayName="Tableau2210" ref="F1:O10" totalsRowShown="0">
+  <autoFilter ref="F1:O10" xr:uid="{4706B194-EB46-4EE1-B9C3-ED64E3DBE6C0}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{3D5FB965-748A-4682-819A-7C021656DB4B}" name="distance matrix"/>
+    <tableColumn id="2" xr3:uid="{D2830664-1CF7-4092-83AA-C6F490C779B9}" name="1">
+      <calculatedColumnFormula>SQRT((C$2-C2)^2+(D$2-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1D24240D-4ADC-4658-A9B7-E7FD30F8D0AF}" name="2">
+      <calculatedColumnFormula>SQRT((C$3-C2)^2+(D$3-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{44B63950-AB99-4904-9DFD-23624B841A4C}" name="3">
+      <calculatedColumnFormula>SQRT((C$4-C2)^2+(D$4-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{EB05B097-B756-41BD-AC4E-E4605B94E3B8}" name="4">
+      <calculatedColumnFormula>SQRT((C$5-C2)^2+(D$5-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{DAF7D4B3-A10A-4D91-B992-DF6CC17B4D43}" name="5">
+      <calculatedColumnFormula>SQRT((C$6-C2)^2+(D$6-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{134AADDC-B1B3-47FF-9DD5-16E844F4581A}" name="6">
+      <calculatedColumnFormula>SQRT((C$7-C2)^2+(D$7-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{2DFA2CA8-203E-4485-A929-F9DEDB87CA57}" name="D1" dataDxfId="2">
+      <calculatedColumnFormula>SQRT((C$8-C2)^2+(D$8-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{BE6BFF67-BE2B-46BF-A388-CBD6180BC5BB}" name="D2" dataDxfId="1">
+      <calculatedColumnFormula>SQRT((C$9-C2)^2+(D$9-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{D123EDFA-A0B6-4911-A939-D20DA17ECEF6}" name="D3" dataDxfId="0">
+      <calculatedColumnFormula>SQRT((C$10-C2)^2+(D$10-D2)^2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{37EE6B2A-0C17-4839-891A-D7FA3A70B0BA}" name="Tableau3511" displayName="Tableau3511" ref="B1:D10" totalsRowShown="0">
+  <autoFilter ref="B1:D10" xr:uid="{23FEA744-B7A0-4AB4-BA8E-3D1EC4BABB72}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{604E823C-CC84-4E66-97EF-26BDACED2110}" name="Coordonnées"/>
+    <tableColumn id="2" xr3:uid="{CF5787E3-C900-40E1-A1DA-132471B3917B}" name="x"/>
+    <tableColumn id="3" xr3:uid="{4E8C623D-1EA9-43E1-8D35-1E441DA8E401}" name="y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1276,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891FCA0B-77D4-458A-B238-39F87761B2B1}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1325,7 +1656,7 @@
       </c>
       <c r="N1" s="2">
         <f>SUMPRODUCT(G2:L7,B10:G15)</f>
-        <v>8.1925824035672523</v>
+        <v>9.3851648071345046</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1354,7 +1685,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I7" si="2">SQRT((C$4-C2)^2+(D$4-D2)^2)</f>
-        <v>5.2201532544552753</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J7" si="3">SQRT((C$5-C2)^2+(D$5-D2)^2)</f>
@@ -1392,7 +1723,7 @@
       </c>
       <c r="I3">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="J3">
         <f t="shared" si="3"/>
@@ -1415,21 +1746,21 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>5.2201532544552753</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
@@ -1437,15 +1768,15 @@
       </c>
       <c r="J4">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="K4">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>5.0990195135927845</v>
       </c>
       <c r="L4">
         <f t="shared" si="5"/>
-        <v>2.5495097567963922</v>
+        <v>2.6925824035672519</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1471,7 +1802,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="J5">
         <f t="shared" si="3"/>
@@ -1515,7 +1846,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>5.0990195135927845</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
@@ -1559,7 +1890,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>2.5495097567963922</v>
+        <v>2.6925824035672519</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
@@ -1627,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -1636,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <f>SUM(B10:G10)</f>
@@ -1660,13 +1991,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1690,13 +2021,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="6"/>
@@ -1720,10 +2051,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="6"/>
@@ -1744,13 +2075,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3">
         <f>SUM(B14:G14)</f>
@@ -1894,15 +2225,15 @@
       </c>
       <c r="B30">
         <f>D11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="6">
         <f>SUM(A30,B30)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <f>SUM(G10,G11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1926,11 +2257,11 @@
       </c>
       <c r="B32">
         <f>F11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1940,11 +2271,11 @@
       </c>
       <c r="B33">
         <f>E12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1964,15 +2295,2425 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>E14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <f>F13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="6">
         <f t="shared" si="8"/>
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D684BB79-7551-4D82-B7D1-7ED44D6CB47C}">
+  <dimension ref="A1:U48"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="12" max="12" width="11.7890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="8">
+        <f>SUMPRODUCT(G2:O10,L35:T43)</f>
+        <v>78.065667847828223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <f>SQRT((C$2-C2)^2+(D$2-D2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SQRT((C$3-C2)^2+(D$3-D2)^2)</f>
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I7" si="0">SQRT((C$4-C2)^2+(D$4-D2)^2)</f>
+        <v>41.231056256176608</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J7" si="1">SQRT((C$5-C2)^2+(D$5-D2)^2)</f>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K7" si="2">SQRT((C$6-C2)^2+(D$6-D2)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f>SQRT((C$7-C2)^2+(D$7-D2)^2)</f>
+        <v>43.416586692184822</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M10" si="3">SQRT((C$8-C2)^2+(D$8-D2)^2)</f>
+        <v>11.180339887498949</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N10" si="4">SQRT((C$9-C2)^2+(D$9-D2)^2)</f>
+        <v>21.189620100417091</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O10" si="5">SQRT((C$10-C2)^2+(D$10-D2)^2)</f>
+        <v>39.293765408776999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="6">SQRT((C$2-C3)^2+(D$2-D3)^2)</f>
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="7">SQRT((C$3-C3)^2+(D$3-D3)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>29.732137494637012</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>30.463092423455635</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="2"/>
+        <v>12.165525060596439</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="8">SQRT((C$7-C3)^2+(D$7-D3)^2)</f>
+        <v>31.953090617340916</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="4"/>
+        <v>10.63014581273465</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="5"/>
+        <v>27.856776554368238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>-10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="6"/>
+        <v>41.231056256176608</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="7"/>
+        <v>29.732137494637012</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="8"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>30.083217912982647</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>-12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="6"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="7"/>
+        <v>30.463092423455635</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>42.379240200834182</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="8"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>30.675723300355934</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>20.615528128088304</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>12.165525060596439</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>42.379240200834182</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="8"/>
+        <v>43.965895873961216</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>11.704699910719626</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>21.931712199461309</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>39.849717690342551</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>-11</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="6"/>
+        <v>43.416586692184822</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="7"/>
+        <v>31.953090617340916</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>43.965895873961216</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>32.280024783137947</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>22.360679774997898</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7">
+        <f>IF(R5=R6,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="6"/>
+        <v>11.180339887498949</v>
+      </c>
+      <c r="H8">
+        <f>SQRT((C$3-C8)^2+(D$3-D8)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I8">
+        <f>SQRT((C$4-C8)^2+(D$4-D8)^2)</f>
+        <v>30.083217912982647</v>
+      </c>
+      <c r="J8">
+        <f>SQRT((C$5-C8)^2+(D$5-D8)^2)</f>
+        <v>30.675723300355934</v>
+      </c>
+      <c r="K8">
+        <f>SQRT((C$6-C8)^2+(D$6-D8)^2)</f>
+        <v>11.704699910719626</v>
+      </c>
+      <c r="L8">
+        <f>SQRT((C$7-C8)^2+(D$7-D8)^2)</f>
+        <v>32.280024783137947</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>10.295630140987001</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>28.160255680657446</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8">
+        <f>R6-R7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>-7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>21.189620100417091</v>
+      </c>
+      <c r="H9">
+        <f>SQRT((C$3-C9)^2+(D$3-D9)^2)</f>
+        <v>10.63014581273465</v>
+      </c>
+      <c r="I9">
+        <f>SQRT((C$4-C9)^2+(D$4-D9)^2)</f>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="J9">
+        <f>SQRT((C$5-C9)^2+(D$5-D9)^2)</f>
+        <v>20.615528128088304</v>
+      </c>
+      <c r="K9">
+        <f>SQRT((C$6-C9)^2+(D$6-D9)^2)</f>
+        <v>21.931712199461309</v>
+      </c>
+      <c r="L9">
+        <f>SQRT((C$7-C9)^2+(D$7-D9)^2)</f>
+        <v>22.360679774997898</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>10.295630140987001</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>18.248287590894659</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>-10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10">
+        <f>SQRT((C$2-C10)^2+(D$2-D10)^2)</f>
+        <v>39.293765408776999</v>
+      </c>
+      <c r="H10">
+        <f>SQRT((C$3-C10)^2+(D$3-D10)^2)</f>
+        <v>27.856776554368238</v>
+      </c>
+      <c r="I10">
+        <f>SQRT((C$4-C10)^2+(D$4-D10)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f>SQRT((C$5-C10)^2+(D$5-D10)^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="K10">
+        <f>SQRT((C$6-C10)^2+(D$6-D10)^2)</f>
+        <v>39.849717690342551</v>
+      </c>
+      <c r="L10">
+        <f>SQRT((C$7-C10)^2+(D$7-D10)^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>28.160255680657446</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <f>L35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <f>M36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <f>N37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <f>O38</f>
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <f>P39</f>
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <f>Q40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <f>R41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <f>S42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <f>T43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <f>P40</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f>Q39</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <f>SUM(A30,B30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R32">
+        <f>R33*R$6</f>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f>S33*R$6</f>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f>T33*R$6</f>
+        <v>4</v>
+      </c>
+      <c r="U32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <f>SUM(R33:T33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K34" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" t="s">
+        <v>41</v>
+      </c>
+      <c r="N34" t="s">
+        <v>42</v>
+      </c>
+      <c r="O34" t="s">
+        <v>43</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>2</v>
+      </c>
+      <c r="R34" t="s">
+        <v>44</v>
+      </c>
+      <c r="S34" t="s">
+        <v>45</v>
+      </c>
+      <c r="T34" t="s">
+        <v>46</v>
+      </c>
+      <c r="U34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K35" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="U35" s="5">
+        <f>SUM(L35:T35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K36" t="s">
+        <v>41</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1</v>
+      </c>
+      <c r="U36" s="5">
+        <f t="shared" ref="U36:U38" si="9">SUM(L36:T36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K37" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="U37" s="5">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K38" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
+      <c r="U38" s="5">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1">
+        <v>1</v>
+      </c>
+      <c r="U39" s="3">
+        <f t="shared" ref="U36:U43" si="10">SUM(L39:T39)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1">
+        <v>0</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+      <c r="T40" s="1">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K41" t="s">
+        <v>44</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1">
+        <v>0</v>
+      </c>
+      <c r="U41" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K42" t="s">
+        <v>45</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1">
+        <v>0</v>
+      </c>
+      <c r="U42" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K43" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <v>0</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+      <c r="T43" s="1">
+        <v>0</v>
+      </c>
+      <c r="U43" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="K44" t="s">
+        <v>51</v>
+      </c>
+      <c r="L44" s="5">
+        <f>SUM(L35:L43)</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <f t="shared" ref="M44:O44" si="11">SUM(M35:M43)</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <f>SUM(P35:P43)</f>
+        <v>1</v>
+      </c>
+      <c r="Q44" s="3">
+        <f>SUM(Q35:Q43)</f>
+        <v>1</v>
+      </c>
+      <c r="R44" s="4">
+        <f t="shared" ref="M44:T44" si="12">SUM(R35:R43)</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="4">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="11:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R48">
+        <f>SUM(R35:R38)</f>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <f>SUM(S35:S38)</f>
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <f>SUM(T35:T38)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC95D18-69E5-44F4-B219-1B407DEDC463}">
+  <dimension ref="A1:U53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="12" max="12" width="11.7890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="8">
+        <f>SUMPRODUCT(G2:O10,L35:T43)</f>
+        <v>78.065667847828223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>SQRT((C$2-C2)^2+(D$2-D2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SQRT((C$3-C2)^2+(D$3-D2)^2)</f>
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I7" si="0">SQRT((C$4-C2)^2+(D$4-D2)^2)</f>
+        <v>41.231056256176608</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J7" si="1">SQRT((C$5-C2)^2+(D$5-D2)^2)</f>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K7" si="2">SQRT((C$6-C2)^2+(D$6-D2)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f>SQRT((C$7-C2)^2+(D$7-D2)^2)</f>
+        <v>43.416586692184822</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M10" si="3">SQRT((C$8-C2)^2+(D$8-D2)^2)</f>
+        <v>11.180339887498949</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N10" si="4">SQRT((C$9-C2)^2+(D$9-D2)^2)</f>
+        <v>21.189620100417091</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2:O10" si="5">SQRT((C$10-C2)^2+(D$10-D2)^2)</f>
+        <v>39.293765408776999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="6">SQRT((C$2-C3)^2+(D$2-D3)^2)</f>
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="7">SQRT((C$3-C3)^2+(D$3-D3)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>29.732137494637012</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>30.463092423455635</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="2"/>
+        <v>12.165525060596439</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="8">SQRT((C$7-C3)^2+(D$7-D3)^2)</f>
+        <v>31.953090617340916</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="3"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="4"/>
+        <v>10.63014581273465</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="5"/>
+        <v>27.856776554368238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>-10</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="6"/>
+        <v>41.231056256176608</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="7"/>
+        <v>29.732137494637012</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="8"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>30.083217912982647</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="4"/>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>-12</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="6"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="7"/>
+        <v>30.463092423455635</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>42.379240200834182</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="8"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>30.675723300355934</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>20.615528128088304</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>12.165525060596439</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>41.761226035642203</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>42.379240200834182</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="8"/>
+        <v>43.965895873961216</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>11.704699910719626</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>21.931712199461309</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>39.849717690342551</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="9">
+        <f>SUM(E2:E7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>-11</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="6"/>
+        <v>43.416586692184822</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="7"/>
+        <v>31.953090617340916</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>43.965895873961216</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>32.280024783137947</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>22.360679774997898</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7">
+        <f>IF(R5=R6,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="6"/>
+        <v>11.180339887498949</v>
+      </c>
+      <c r="H8">
+        <f>SQRT((C$3-C8)^2+(D$3-D8)^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I8">
+        <f>SQRT((C$4-C8)^2+(D$4-D8)^2)</f>
+        <v>30.083217912982647</v>
+      </c>
+      <c r="J8">
+        <f>SQRT((C$5-C8)^2+(D$5-D8)^2)</f>
+        <v>30.675723300355934</v>
+      </c>
+      <c r="K8">
+        <f>SQRT((C$6-C8)^2+(D$6-D8)^2)</f>
+        <v>11.704699910719626</v>
+      </c>
+      <c r="L8">
+        <f>SQRT((C$7-C8)^2+(D$7-D8)^2)</f>
+        <v>32.280024783137947</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>10.295630140987001</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>28.160255680657446</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8">
+        <f>R6-R7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>-7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>21.189620100417091</v>
+      </c>
+      <c r="H9">
+        <f>SQRT((C$3-C9)^2+(D$3-D9)^2)</f>
+        <v>10.63014581273465</v>
+      </c>
+      <c r="I9">
+        <f>SQRT((C$4-C9)^2+(D$4-D9)^2)</f>
+        <v>20.223748416156685</v>
+      </c>
+      <c r="J9">
+        <f>SQRT((C$5-C9)^2+(D$5-D9)^2)</f>
+        <v>20.615528128088304</v>
+      </c>
+      <c r="K9">
+        <f>SQRT((C$6-C9)^2+(D$6-D9)^2)</f>
+        <v>21.931712199461309</v>
+      </c>
+      <c r="L9">
+        <f>SQRT((C$7-C9)^2+(D$7-D9)^2)</f>
+        <v>22.360679774997898</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>10.295630140987001</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>18.248287590894659</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>-10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10">
+        <f>SQRT((C$2-C10)^2+(D$2-D10)^2)</f>
+        <v>39.293765408776999</v>
+      </c>
+      <c r="H10">
+        <f>SQRT((C$3-C10)^2+(D$3-D10)^2)</f>
+        <v>27.856776554368238</v>
+      </c>
+      <c r="I10">
+        <f>SQRT((C$4-C10)^2+(D$4-D10)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f>SQRT((C$5-C10)^2+(D$5-D10)^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="K10">
+        <f>SQRT((C$6-C10)^2+(D$6-D10)^2)</f>
+        <v>39.849717690342551</v>
+      </c>
+      <c r="L10">
+        <f>SQRT((C$7-C10)^2+(D$7-D10)^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>28.160255680657446</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <f>L35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <f>M36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <f>N37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <f>O38</f>
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <f>P39</f>
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <f>Q40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <f>R41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <f>S42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <f>T43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="10">
+        <f>L36</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f>M35</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <f>SUM(A30,B30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10">
+        <f t="shared" ref="A31:A34" si="9">L37</f>
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <f>N35</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" ref="C31:C44" si="10">SUM(A31,B31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <f>O35</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f>R33*R$6</f>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f>S33*R$6</f>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f>T33*R$6</f>
+        <v>1</v>
+      </c>
+      <c r="U32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <f>P35</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <f>SUM(R33:T33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <f>Q35</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
+      <c r="P34">
+        <v>5</v>
+      </c>
+      <c r="Q34">
+        <v>6</v>
+      </c>
+      <c r="R34" t="s">
+        <v>44</v>
+      </c>
+      <c r="S34" t="s">
+        <v>45</v>
+      </c>
+      <c r="T34" t="s">
+        <v>46</v>
+      </c>
+      <c r="U34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="11">
+        <f>M37</f>
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <f>N36</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>57</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <f t="shared" ref="U35:U43" si="11">SUM(L35:T35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="11">
+        <f t="shared" ref="A36:A38" si="12">M38</f>
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <f>O36</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <f>P36</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+      <c r="U37" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <f>Q36</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
+      <c r="U38" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="3">
+        <f>N38</f>
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <f>O37</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1">
+        <v>1</v>
+      </c>
+      <c r="U39" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="3">
+        <f t="shared" ref="A40:A41" si="13">N39</f>
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <f>P37</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>6</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1">
+        <v>0</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+      <c r="T40" s="1">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <f>Q37</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>44</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1">
+        <v>0</v>
+      </c>
+      <c r="U41" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="12">
+        <f>O39</f>
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <f>P38</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
+        <v>45</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1">
+        <v>0</v>
+      </c>
+      <c r="U42" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="12">
+        <f>O40</f>
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <f>Q38</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K43" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <v>0</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+      <c r="T43" s="1">
+        <v>0</v>
+      </c>
+      <c r="U43" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <f>P40</f>
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <f>Q39</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>51</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" ref="L44:O44" si="14">SUM(L35:L43)</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <f>SUM(P35:P43)</f>
+        <v>1</v>
+      </c>
+      <c r="Q44" s="3">
+        <f>SUM(Q35:Q43)</f>
+        <v>1</v>
+      </c>
+      <c r="R44" s="4">
+        <f t="shared" ref="R44:T44" si="15">SUM(R35:R43)</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="4">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="R48">
+        <f>SUM(R35:R38)</f>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <f>SUM(S35:S38)</f>
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <f>SUM(T35:T38)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="11:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="K50" t="s">
+        <v>59</v>
+      </c>
+      <c r="L50">
+        <f>1 - E2</f>
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <f>1 - E3</f>
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <f>1 - E4</f>
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <f>1 - E5</f>
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <f>1-E6</f>
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <f>1-E7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="11:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="K53" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remaining constraint to case1f
</commit_message>
<xml_diff>
--- a/case1.xlsx
+++ b/case1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8775" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8775" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Case1a" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="solver_adj" localSheetId="5" hidden="1">Case1f!$L$22:$Q$22,Case1f!$R$33:$T$33,Case1f!$L$35:$T$43,Case1f!$E$2:$E$7,Case1f!$U$4,Case1f!$R$56:$T$61</definedName>
     <definedName name="solver_adj_ob" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_adj_ob1" localSheetId="5" hidden="1">1</definedName>
-    <definedName name="solver_adj1" localSheetId="5" hidden="1">Case1f!$T$23</definedName>
+    <definedName name="solver_adj1" localSheetId="5" hidden="1">Case1f!$R$46:$T$51</definedName>
     <definedName name="solver_cha" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc1" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc10" localSheetId="5" hidden="1">0</definedName>
@@ -55,7 +55,14 @@
     <definedName name="solver_chc24" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc25" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc26" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc27" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc28" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc29" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc3" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc30" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc31" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc32" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chc33" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc4" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc5" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chc6" localSheetId="5" hidden="1">0</definedName>
@@ -82,7 +89,14 @@
     <definedName name="solver_chp24" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp25" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp26" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp27" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp28" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp29" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp3" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp30" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp31" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp32" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_chp33" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp4" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp5" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_chp6" localSheetId="5" hidden="1">0</definedName>
@@ -109,7 +123,14 @@
     <definedName name="solver_cir24" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir25" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir26" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir27" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir28" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir29" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir3" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir30" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir31" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir32" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_cir33" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir4" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir5" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_cir6" localSheetId="5" hidden="1">1</definedName>
@@ -136,7 +157,14 @@
     <definedName name="solver_con24" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con25" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con26" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con27" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con28" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con29" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con3" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con30" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con31" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con32" localSheetId="5" hidden="1">" "</definedName>
+    <definedName name="solver_con33" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con4" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con5" localSheetId="5" hidden="1">" "</definedName>
     <definedName name="solver_con6" localSheetId="5" hidden="1">" "</definedName>
@@ -198,7 +226,14 @@
     <definedName name="solver_lhs_ob24" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob25" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob26" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob27" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob28" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob29" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob3" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob30" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob31" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob32" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_lhs_ob33" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob4" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob5" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_lhs_ob6" localSheetId="5" hidden="1">0</definedName>
@@ -252,12 +287,19 @@
     <definedName name="solver_lhs24" localSheetId="5" hidden="1">Case1f!$U$41:$U$43</definedName>
     <definedName name="solver_lhs25" localSheetId="5" hidden="1">Case1f!$U$5</definedName>
     <definedName name="solver_lhs26" localSheetId="5" hidden="1">Case1f!$X$35:$AC$40</definedName>
+    <definedName name="solver_lhs27" localSheetId="5" hidden="1">Case1f!$R$46:$T$51</definedName>
+    <definedName name="solver_lhs28" localSheetId="5" hidden="1">Case1f!$R$46:$T$51</definedName>
+    <definedName name="solver_lhs29" localSheetId="5" hidden="1">Case1f!$R$46:$R$51</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Case1a!$B$16</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Case1b!$B$16:$C$16</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">Case1c!$L$35:$T$43</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">Case1d!$E$2:$E$7</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">Case1e!$E$2:$E$7</definedName>
     <definedName name="solver_lhs3" localSheetId="5" hidden="1">Case1f!$E$2:$E$7</definedName>
+    <definedName name="solver_lhs30" localSheetId="5" hidden="1">Case1f!$S$46:$S$51</definedName>
+    <definedName name="solver_lhs31" localSheetId="5" hidden="1">Case1f!$T$46:$T$51</definedName>
+    <definedName name="solver_lhs32" localSheetId="5" hidden="1">Case1f!$R$46:$T$51</definedName>
+    <definedName name="solver_lhs33" localSheetId="5" hidden="1">Case1f!$R$52:$T$52</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Case1a!$C$16:$F$16</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">Case1b!$C$30:$C$35</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">Case1c!$L$44:$O$44</definedName>
@@ -340,7 +382,7 @@
     <definedName name="solver_num" localSheetId="2" hidden="1">11</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">13</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">17</definedName>
-    <definedName name="solver_num" localSheetId="5" hidden="1">26</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">33</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
@@ -389,7 +431,14 @@
     <definedName name="solver_reco24" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco25" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco26" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco27" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco28" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco29" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco3" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco30" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco31" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco32" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_reco33" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco4" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco5" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_reco6" localSheetId="5" hidden="1">0</definedName>
@@ -443,12 +492,19 @@
     <definedName name="solver_rel24" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rel25" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel26" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel27" localSheetId="5" hidden="1">5</definedName>
+    <definedName name="solver_rel28" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel29" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">5</definedName>
     <definedName name="solver_rel3" localSheetId="5" hidden="1">5</definedName>
+    <definedName name="solver_rel30" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel31" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel32" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel33" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">2</definedName>
@@ -529,16 +585,20 @@
     <definedName name="solver_rhs20" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rhs21" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rhs22" localSheetId="5" hidden="1">Case1f!$U$2</definedName>
-    <definedName name="solver_rhs23" localSheetId="5" hidden="1">binaire</definedName>
     <definedName name="solver_rhs24" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rhs25" localSheetId="5" hidden="1">Case1f!$U$2</definedName>
     <definedName name="solver_rhs26" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs28" localSheetId="5" hidden="1">Case1f!$R$35:$T$40</definedName>
+    <definedName name="solver_rhs29" localSheetId="5" hidden="1">Case1f!$E$2:$E$7</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">binaire</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">binaire</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">binaire</definedName>
-    <definedName name="solver_rhs3" localSheetId="5" hidden="1">binaire</definedName>
+    <definedName name="solver_rhs30" localSheetId="5" hidden="1">Case1f!$E$2:$E$7</definedName>
+    <definedName name="solver_rhs31" localSheetId="5" hidden="1">Case1f!$E$2:$E$7</definedName>
+    <definedName name="solver_rhs32" localSheetId="5" hidden="1">Case1f!$V$46:$X$51</definedName>
+    <definedName name="solver_rhs33" localSheetId="5" hidden="1">Case1f!$R$8</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
@@ -550,7 +610,6 @@
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">Case1d!$L$50:$Q$50</definedName>
     <definedName name="solver_rhs5" localSheetId="4" hidden="1">entier</definedName>
-    <definedName name="solver_rhs5" localSheetId="5" hidden="1">entier</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="1" hidden="1">Case1b!$N$6</definedName>
     <definedName name="solver_rhs6" localSheetId="2" hidden="1">binaire</definedName>
@@ -562,7 +621,6 @@
     <definedName name="solver_rhs7" localSheetId="2" hidden="1">Case1c!$R$32:$T$32</definedName>
     <definedName name="solver_rhs7" localSheetId="3" hidden="1">Case1d!$R$32:$T$32</definedName>
     <definedName name="solver_rhs7" localSheetId="4" hidden="1">binaire</definedName>
-    <definedName name="solver_rhs7" localSheetId="5" hidden="1">binaire</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs8" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs8" localSheetId="2" hidden="1">Case1c!$R$8</definedName>
@@ -574,13 +632,12 @@
     <definedName name="solver_rhs9" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs9" localSheetId="3" hidden="1">Case1d!$R$5</definedName>
     <definedName name="solver_rhs9" localSheetId="4" hidden="1">binaire</definedName>
-    <definedName name="solver_rhs9" localSheetId="5" hidden="1">binaire</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
@@ -608,7 +665,14 @@
     <definedName name="solver_rxc24" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc25" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc26" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc27" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc28" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc29" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc3" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc30" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc31" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc32" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rxc33" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc4" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc5" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_rxc6" localSheetId="5" hidden="1">1</definedName>
@@ -680,7 +744,7 @@
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">17</definedName>
     <definedName name="solver_vir" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_vir1" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_vol" localSheetId="5" hidden="1">0</definedName>
@@ -702,7 +766,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="77">
   <si>
     <t>distance matrix</t>
   </si>
@@ -927,6 +991,12 @@
   </si>
   <si>
     <t>Commentaire: Linéairisation des 2 contraintes non linéaires (case1d)</t>
+  </si>
+  <si>
+    <t>sum (ai bij)</t>
+  </si>
+  <si>
+    <t>ai*bij</t>
   </si>
 </sst>
 </file>
@@ -7197,8 +7267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7258,7 +7328,7 @@
       </c>
       <c r="R1" s="8">
         <f>SUMPRODUCT(G2:O10,L35:T43)</f>
-        <v>1006.1760051740979</v>
+        <v>1014.1342524532591</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -7294,7 +7364,7 @@
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J7" si="1">SQRT((C$5-C2)^2+(D$5-D2)^2)</f>
-        <v>960.07499707054137</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K7" si="2">SQRT((C$6-C2)^2+(D$6-D2)^2)</f>
@@ -7321,7 +7391,7 @@
       </c>
       <c r="U2">
         <f>R5-R6</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -7354,7 +7424,7 @@
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>30.463092423455635</v>
+        <v>988.07287180652827</v>
       </c>
       <c r="K3">
         <f t="shared" si="2"/>
@@ -7417,7 +7487,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>960.00208333107275</v>
       </c>
       <c r="K4">
         <f t="shared" si="2"/>
@@ -7457,28 +7527,28 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>1000</v>
       </c>
       <c r="D5">
         <v>-12</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
         <f t="shared" si="6"/>
-        <v>960.07499707054137</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
-        <v>30.463092423455635</v>
+        <v>988.07287180652827</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>960.00208333107275</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
@@ -7486,23 +7556,23 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>42.379240200834182</v>
+        <v>1000.0979951984706</v>
       </c>
       <c r="L5">
         <f t="shared" si="8"/>
-        <v>2.2360679774997898</v>
+        <v>958.0005219205259</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>960.05208192055909</v>
+        <v>10</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>960.01302074503133</v>
+        <v>5</v>
       </c>
       <c r="O5">
         <f t="shared" si="5"/>
-        <v>960.00208333107275</v>
+        <v>2</v>
       </c>
       <c r="Q5" t="s">
         <v>36</v>
@@ -7548,7 +7618,7 @@
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>42.379240200834182</v>
+        <v>1000.0979951984706</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
@@ -7575,7 +7645,7 @@
       </c>
       <c r="R6" s="9">
         <f>SUM(E2:E7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -7608,7 +7678,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>2.2360679774997898</v>
+        <v>958.0005219205259</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
@@ -7665,7 +7735,7 @@
       </c>
       <c r="J8">
         <f>SQRT((C$5-C8)^2+(D$5-D8)^2)</f>
-        <v>960.05208192055909</v>
+        <v>10</v>
       </c>
       <c r="K8">
         <f>SQRT((C$6-C8)^2+(D$6-D8)^2)</f>
@@ -7692,7 +7762,7 @@
       </c>
       <c r="R8">
         <f>R6-U4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -7722,7 +7792,7 @@
       </c>
       <c r="J9">
         <f>SQRT((C$5-C9)^2+(D$5-D9)^2)</f>
-        <v>960.01302074503133</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <f>SQRT((C$6-C9)^2+(D$6-D9)^2)</f>
@@ -7772,7 +7842,7 @@
       </c>
       <c r="J10">
         <f>SQRT((C$5-C10)^2+(D$5-D10)^2)</f>
-        <v>960.00208333107275</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f>SQRT((C$6-C10)^2+(D$6-D10)^2)</f>
@@ -7839,10 +7909,10 @@
         <v>2</v>
       </c>
       <c r="N22" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P22" s="1">
         <v>1</v>
@@ -7862,9 +7932,6 @@
       <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -7881,11 +7948,11 @@
       </c>
       <c r="N24">
         <f>$N$22</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O24">
         <f>$O$22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P24">
         <f>$P$22</f>
@@ -7939,11 +8006,11 @@
       </c>
       <c r="N25">
         <f t="shared" ref="N25:N29" si="12">$N$22</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O25">
         <f t="shared" ref="O25:O29" si="13">$O$22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P25">
         <f t="shared" ref="P25:P29" si="14">$P$22</f>
@@ -7997,11 +8064,11 @@
       </c>
       <c r="N26">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O26">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P26">
         <f t="shared" si="14"/>
@@ -8013,31 +8080,31 @@
       </c>
       <c r="S26" s="13">
         <f>N22</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T26">
         <f>$N$22</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U26">
         <f t="shared" ref="U26:Y26" si="17">$N$22</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V26">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W26">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X26">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y26">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -8055,11 +8122,11 @@
       </c>
       <c r="N27">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O27">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P27">
         <f t="shared" si="14"/>
@@ -8071,31 +8138,31 @@
       </c>
       <c r="S27" s="13">
         <f>O22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T27">
         <f>$O$22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U27">
         <f t="shared" ref="U27:Y27" si="18">$O$22</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V27">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W27">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X27">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y27">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -8109,11 +8176,11 @@
       </c>
       <c r="N28">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O28">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P28">
         <f t="shared" si="14"/>
@@ -8166,11 +8233,11 @@
       </c>
       <c r="N29">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O29">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P29">
         <f t="shared" si="14"/>
@@ -8252,7 +8319,7 @@
       </c>
       <c r="R32">
         <f>R33*R$6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S32">
         <f>S33*R$6</f>
@@ -8260,7 +8327,7 @@
       </c>
       <c r="T32">
         <f>T33*R$6</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U32" t="s">
         <v>52</v>
@@ -8280,13 +8347,13 @@
         <v>0</v>
       </c>
       <c r="R33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" s="1">
         <v>0</v>
       </c>
       <c r="T33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
         <f>SUM(R33:T33)</f>
@@ -8375,13 +8442,13 @@
         <v>0</v>
       </c>
       <c r="R35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" s="1">
         <v>0</v>
       </c>
       <c r="T35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" s="3">
         <f t="shared" ref="U35:U43" si="23">SUM(L35:T35)</f>
@@ -8397,11 +8464,11 @@
       </c>
       <c r="Z35">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA35">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB35">
         <f t="shared" si="24"/>
@@ -8469,11 +8536,11 @@
       </c>
       <c r="Z36">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA36">
         <f t="shared" si="24"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB36">
         <f t="shared" si="24"/>
@@ -8510,13 +8577,13 @@
         <v>0</v>
       </c>
       <c r="O37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="1">
         <v>0</v>
       </c>
       <c r="Q37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="1">
         <v>0</v>
@@ -8533,11 +8600,11 @@
       </c>
       <c r="X37">
         <f t="shared" si="26"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Y37">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z37">
         <f t="shared" si="24"/>
@@ -8545,15 +8612,15 @@
       </c>
       <c r="AA37">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB37">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC37">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -8588,7 +8655,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R38" s="1">
         <v>0</v>
@@ -8597,7 +8664,7 @@
         <v>0</v>
       </c>
       <c r="T38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" s="3">
         <f t="shared" si="23"/>
@@ -8605,15 +8672,15 @@
       </c>
       <c r="X38">
         <f t="shared" si="26"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Y38">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z38">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AA38">
         <f t="shared" si="24"/>
@@ -8621,11 +8688,11 @@
       </c>
       <c r="AB38">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC38">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
@@ -8635,11 +8702,11 @@
       </c>
       <c r="B39">
         <f>O37</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39">
         <v>5</v>
@@ -8685,11 +8752,11 @@
       </c>
       <c r="Z39">
         <f t="shared" si="24"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AA39">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AB39">
         <f t="shared" si="24"/>
@@ -8735,13 +8802,13 @@
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" s="1">
         <v>0</v>
       </c>
       <c r="T40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" s="3">
         <f t="shared" si="23"/>
@@ -8757,11 +8824,11 @@
       </c>
       <c r="Z40">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA40">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB40">
         <f t="shared" si="24"/>
@@ -8779,11 +8846,11 @@
       </c>
       <c r="B41">
         <f>Q37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" t="s">
         <v>44</v>
@@ -8875,11 +8942,11 @@
       </c>
       <c r="B43">
         <f>Q38</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" t="s">
         <v>46</v>
@@ -8946,7 +9013,7 @@
       </c>
       <c r="O44" s="3">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" s="3">
         <f>SUM(P35:P43)</f>
@@ -8958,7 +9025,7 @@
       </c>
       <c r="R44" s="4">
         <f t="shared" ref="R44:T44" si="29">SUM(R35:R43)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S44" s="4">
         <f t="shared" si="29"/>
@@ -8966,32 +9033,106 @@
       </c>
       <c r="T44" s="4">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q46" t="s">
+        <v>76</v>
+      </c>
+      <c r="R46" s="1">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1">
+        <v>1</v>
+      </c>
+      <c r="V46">
+        <f>R35+$E2-1</f>
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <f t="shared" ref="W46:X51" si="30">S35+$E2-1</f>
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="30"/>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="R47" t="s">
-        <v>39</v>
+      <c r="R47" s="1">
+        <v>0</v>
+      </c>
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <f t="shared" ref="V47:V51" si="31">R36+$E3-1</f>
+        <v>-1</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="30"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="R48">
-        <f>SUM(R35:R38)</f>
-        <v>1</v>
-      </c>
-      <c r="S48">
-        <f>SUM(S35:S38)</f>
-        <v>0</v>
-      </c>
-      <c r="T48">
-        <f>SUM(T35:T38)</f>
-        <v>0</v>
+      <c r="R48" s="1">
+        <v>0</v>
+      </c>
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="30"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>74</v>
       </c>
+      <c r="R49" s="1">
+        <v>0</v>
+      </c>
+      <c r="S49" s="1">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1">
+        <v>1</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <f>T38+$E5-1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K50" t="s">
@@ -9011,7 +9152,7 @@
       </c>
       <c r="O50">
         <f>1 - E5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50">
         <f>1-E6</f>
@@ -9020,6 +9161,67 @@
       <c r="Q50">
         <f>1-E7</f>
         <v>1</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R51" s="1">
+        <v>0</v>
+      </c>
+      <c r="S51" s="1">
+        <v>0</v>
+      </c>
+      <c r="T51" s="1">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="31"/>
+        <v>-1</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="30"/>
+        <v>-1</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Q52" t="s">
+        <v>75</v>
+      </c>
+      <c r="R52">
+        <f>SUM(R46:R51)</f>
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <f t="shared" ref="S52:T52" si="32">SUM(S46:S51)</f>
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="32"/>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
@@ -9028,15 +9230,15 @@
       </c>
       <c r="R53">
         <f>SUMPRODUCT($E$2:$E$7,R35:R40)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S53">
         <f>SUMPRODUCT($E$2:$E$7,S35:S40)</f>
         <v>0</v>
       </c>
       <c r="T53">
-        <f t="shared" ref="T53" si="30">SUMPRODUCT($E$2:$E$7,T35:T40)</f>
-        <v>0</v>
+        <f t="shared" ref="T53" si="33">SUMPRODUCT($E$2:$E$7,T35:T40)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -9044,17 +9246,17 @@
         <v>67</v>
       </c>
       <c r="R56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S56" s="1">
         <v>0</v>
       </c>
       <c r="T56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V56">
         <f>$R$33+E2 -1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W56">
         <f>$S$33+E2-1</f>
@@ -9062,7 +9264,7 @@
       </c>
       <c r="X56">
         <f>$T$33+E2-1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -9076,16 +9278,16 @@
         <v>0</v>
       </c>
       <c r="V57">
-        <f t="shared" ref="V57:V61" si="31">$R$33+E3 -1</f>
-        <v>0</v>
+        <f t="shared" ref="V57:V61" si="34">$R$33+E3 -1</f>
+        <v>-1</v>
       </c>
       <c r="W57">
-        <f t="shared" ref="W57:W61" si="32">$S$33+E3-1</f>
+        <f t="shared" ref="W57:W61" si="35">$S$33+E3-1</f>
         <v>-1</v>
       </c>
       <c r="X57">
-        <f t="shared" ref="X57:X61" si="33">$T$33+E3-1</f>
-        <v>-1</v>
+        <f t="shared" ref="X57:X61" si="36">$T$33+E3-1</f>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -9099,19 +9301,22 @@
         <v>0</v>
       </c>
       <c r="V58">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="W58">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-1</v>
       </c>
       <c r="X58">
-        <f t="shared" si="33"/>
-        <v>-1</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>39</v>
+      </c>
       <c r="R59" s="1">
         <v>0</v>
       </c>
@@ -9119,42 +9324,54 @@
         <v>0</v>
       </c>
       <c r="T59" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V59">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W59">
-        <f t="shared" si="32"/>
-        <v>-1</v>
+        <f t="shared" si="35"/>
+        <v>0</v>
       </c>
       <c r="X59">
-        <f t="shared" si="33"/>
-        <v>-1</v>
+        <f t="shared" si="36"/>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <f>SUM(R35:R38)</f>
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <f>SUM(S35:S38)</f>
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <f>SUM(T35:T38)</f>
+        <v>2</v>
+      </c>
       <c r="R60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S60" s="1">
         <v>0</v>
       </c>
       <c r="T60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V60">
-        <f t="shared" si="31"/>
-        <v>1</v>
+        <f t="shared" si="34"/>
+        <v>0</v>
       </c>
       <c r="W60">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="X60">
-        <f t="shared" si="33"/>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -9168,16 +9385,16 @@
         <v>0</v>
       </c>
       <c r="V61">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <f t="shared" si="34"/>
+        <v>-1</v>
       </c>
       <c r="W61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>-1</v>
       </c>
       <c r="X61">
-        <f t="shared" si="33"/>
-        <v>-1</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
@@ -9186,15 +9403,15 @@
       </c>
       <c r="R62">
         <f>SUM(R56:R61)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S62">
-        <f t="shared" ref="S62:T62" si="34">SUM(S56:S61)</f>
+        <f t="shared" ref="S62:T62" si="37">SUM(S56:S61)</f>
         <v>0</v>
       </c>
       <c r="T62">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="37"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>